<commit_message>
force excel formula recalc on load.
</commit_message>
<xml_diff>
--- a/public/testmaterial/Auswertungstabelle.xlsx
+++ b/public/testmaterial/Auswertungstabelle.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="13">
   <si>
     <t xml:space="preserve">Auswertungstabelle</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t xml:space="preserve">E=Grp:0-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addition</t>
   </si>
   <si>
     <t xml:space="preserve">B=Zweite Seite</t>
@@ -191,10 +194,10 @@
   <dimension ref="A1:C171"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.32"/>
   </cols>
@@ -263,6 +266,15 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="0" t="e">
+        <f aca="false">B18+B15</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,11 +737,11 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>